<commit_message>
Shifted interferograms to be centered about 0
</commit_message>
<xml_diff>
--- a/compressed_sensing/data/metadata.xlsx
+++ b/compressed_sensing/data/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/compressed_sensing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68D598DB-D94A-4EC3-BBE8-6E939C959609}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D8AD0A3-CE07-49D1-B8B5-AFF577379BF3}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>read noise (% of peak)</t>
+  </si>
+  <si>
+    <t>New normalisation meathod. Ideal (coherent, noiseless) Interferogram peaks are now set to 1.</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>1dmockanderrors3.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors4.csv</t>
   </si>
 </sst>
 </file>
@@ -131,12 +143,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -154,9 +165,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{70A695AD-CD1A-4939-8512-07C2F4E67915}" name="Table3" displayName="Table3" ref="B2:H8" totalsRowShown="0">
-  <autoFilter ref="B2:H8" xr:uid="{70A695AD-CD1A-4939-8512-07C2F4E67915}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{70A695AD-CD1A-4939-8512-07C2F4E67915}" name="Table3" displayName="Table3" ref="B2:H9" totalsRowShown="0">
+  <autoFilter ref="B2:H9" xr:uid="{70A695AD-CD1A-4939-8512-07C2F4E67915}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{EF96EA9C-6A3B-4EEF-9428-6E053DCB30F4}" name="name"/>
     <tableColumn id="2" xr3:uid="{EAF267CD-FA98-4843-86FB-9FCA5C38C1B0}" name="array length (pixels)"/>
@@ -171,9 +186,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B0422EBC-0E69-4D8E-B10C-AB12EDC2789D}" name="Table4" displayName="Table4" ref="B11:K14" totalsRowShown="0">
-  <autoFilter ref="B11:K14" xr:uid="{B0422EBC-0E69-4D8E-B10C-AB12EDC2789D}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B0422EBC-0E69-4D8E-B10C-AB12EDC2789D}" name="Table4" displayName="Table4" ref="B12:L16" totalsRowShown="0">
+  <autoFilter ref="B12:L16" xr:uid="{B0422EBC-0E69-4D8E-B10C-AB12EDC2789D}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{77F589C9-5F6B-46DA-9EEE-F5DBA498B0C1}" name="name"/>
     <tableColumn id="2" xr3:uid="{E2EBA6EE-B0E4-4DBE-AC80-C9B804CE497A}" name="array length (pixels)"/>
     <tableColumn id="3" xr3:uid="{5AB64FD2-8CF1-41A3-883B-744D1261D8F9}" name="pixel pitch (um)"/>
@@ -184,6 +199,7 @@
     <tableColumn id="8" xr3:uid="{D0BFD5E9-72B0-484B-903D-FA5887034A89}" name="incoherance std"/>
     <tableColumn id="9" xr3:uid="{B4A3E234-74BF-4867-B948-7F0DE5726339}" name="read noise (% of peak)"/>
     <tableColumn id="10" xr3:uid="{77B3527C-BD8A-4C2C-8196-7B026BA790D4}" name="averages"/>
+    <tableColumn id="11" xr3:uid="{0756F483-F570-44BA-B1CF-32B491B94B5C}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -452,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K13"/>
+  <dimension ref="B1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,9 +486,10 @@
     <col min="9" max="9" width="17.140625" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +500,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -506,7 +523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -529,7 +546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -552,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -575,7 +592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -598,7 +615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -621,7 +638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -644,87 +661,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>11</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>12</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H12" t="s">
         <v>14</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I12" t="s">
         <v>15</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J12" t="s">
         <v>20</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="L12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>18</v>
-      </c>
-      <c r="C12">
-        <v>400</v>
-      </c>
-      <c r="D12">
-        <v>50</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>60</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <v>20</v>
-      </c>
-      <c r="K12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>19</v>
       </c>
       <c r="C13">
         <v>400</v>
@@ -748,16 +736,88 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K13">
         <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>400</v>
+      </c>
+      <c r="D14">
+        <v>50</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>60</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>400</v>
+      </c>
+      <c r="D15">
+        <v>50</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>60</v>
+      </c>
+      <c r="H15">
+        <v>200</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>20</v>
+      </c>
+      <c r="L15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="B11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>

<commit_message>
Created graphs to show how CS improves with more samples
</commit_message>
<xml_diff>
--- a/compressed_sensing/data/metadata.xlsx
+++ b/compressed_sensing/data/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/compressed_sensing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D8AD0A3-CE07-49D1-B8B5-AFF577379BF3}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F05DCE0-3410-424A-9C0B-4C045A94B456}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -87,9 +87,6 @@
     <t>1dmockanderrors2.csv</t>
   </si>
   <si>
-    <t>read noise (% of peak)</t>
-  </si>
-  <si>
     <t>New normalisation meathod. Ideal (coherent, noiseless) Interferogram peaks are now set to 1.</t>
   </si>
   <si>
@@ -100,6 +97,24 @@
   </si>
   <si>
     <t>1dmockanderrors4.csv</t>
+  </si>
+  <si>
+    <t>read noise (% of coherant peak)</t>
+  </si>
+  <si>
+    <t>1dmockanderrors5.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors6.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors7.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors8.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors9.csv</t>
   </si>
 </sst>
 </file>
@@ -165,10 +180,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{70A695AD-CD1A-4939-8512-07C2F4E67915}" name="Table3" displayName="Table3" ref="B2:H9" totalsRowShown="0">
   <autoFilter ref="B2:H9" xr:uid="{70A695AD-CD1A-4939-8512-07C2F4E67915}"/>
@@ -186,8 +197,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B0422EBC-0E69-4D8E-B10C-AB12EDC2789D}" name="Table4" displayName="Table4" ref="B12:L16" totalsRowShown="0">
-  <autoFilter ref="B12:L16" xr:uid="{B0422EBC-0E69-4D8E-B10C-AB12EDC2789D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B0422EBC-0E69-4D8E-B10C-AB12EDC2789D}" name="Table4" displayName="Table4" ref="B12:L21" totalsRowShown="0">
+  <autoFilter ref="B12:L21" xr:uid="{B0422EBC-0E69-4D8E-B10C-AB12EDC2789D}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{77F589C9-5F6B-46DA-9EEE-F5DBA498B0C1}" name="name"/>
     <tableColumn id="2" xr3:uid="{E2EBA6EE-B0E4-4DBE-AC80-C9B804CE497A}" name="array length (pixels)"/>
@@ -197,7 +208,7 @@
     <tableColumn id="6" xr3:uid="{4BB47892-26E0-4CD1-9413-F2019FBE7E80}" name="theta (arcminutes)"/>
     <tableColumn id="7" xr3:uid="{EE89FD8A-8253-4FA8-A6E9-C11110F0F79F}" name="incoherance waves"/>
     <tableColumn id="8" xr3:uid="{D0BFD5E9-72B0-484B-903D-FA5887034A89}" name="incoherance std"/>
-    <tableColumn id="9" xr3:uid="{B4A3E234-74BF-4867-B948-7F0DE5726339}" name="read noise (% of peak)"/>
+    <tableColumn id="9" xr3:uid="{B4A3E234-74BF-4867-B948-7F0DE5726339}" name="read noise (% of coherant peak)"/>
     <tableColumn id="10" xr3:uid="{77B3527C-BD8A-4C2C-8196-7B026BA790D4}" name="averages"/>
     <tableColumn id="11" xr3:uid="{0756F483-F570-44BA-B1CF-32B491B94B5C}" name="Comments"/>
   </tableColumns>
@@ -468,28 +479,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L16"/>
+  <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +511,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -523,7 +534,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -546,7 +557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -569,7 +580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -592,7 +603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -615,7 +626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -638,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -661,7 +672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
@@ -675,7 +686,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -701,16 +712,16 @@
         <v>15</v>
       </c>
       <c r="J12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K12" t="s">
         <v>16</v>
       </c>
       <c r="L12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>18</v>
       </c>
@@ -742,7 +753,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>19</v>
       </c>
@@ -774,9 +785,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>400</v>
@@ -806,12 +817,199 @@
         <v>20</v>
       </c>
       <c r="L15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>400</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>60</v>
+      </c>
+      <c r="H16">
+        <v>200</v>
+      </c>
+      <c r="I16">
+        <v>1.6</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>400</v>
+      </c>
+      <c r="D17">
+        <v>50</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>60</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>20</v>
+      </c>
+      <c r="K17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18">
+        <v>400</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="G18">
+        <v>60</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>20</v>
+      </c>
+      <c r="K18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19">
+        <v>400</v>
+      </c>
+      <c r="D19">
+        <v>50</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>60</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>20</v>
+      </c>
+      <c r="K19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20">
+        <v>400</v>
+      </c>
+      <c r="D20">
+        <v>50</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>60</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>20</v>
+      </c>
+      <c r="K20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21">
+        <v>400</v>
+      </c>
+      <c r="D21">
+        <v>50</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>0.5</v>
+      </c>
+      <c r="G21">
+        <v>60</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>20</v>
+      </c>
+      <c r="K21">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added width to detectors
</commit_message>
<xml_diff>
--- a/compressed_sensing/data/metadata.xlsx
+++ b/compressed_sensing/data/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/compressed_sensing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F05DCE0-3410-424A-9C0B-4C045A94B456}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE315AF7-4761-4CDA-9D2C-372E6DDCACC3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -87,9 +87,6 @@
     <t>1dmockanderrors2.csv</t>
   </si>
   <si>
-    <t>New normalisation meathod. Ideal (coherent, noiseless) Interferogram peaks are now set to 1.</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -115,6 +112,27 @@
   </si>
   <si>
     <t>1dmockanderrors9.csv</t>
+  </si>
+  <si>
+    <t>484 runs for 5%</t>
+  </si>
+  <si>
+    <t>27 runs for 5%</t>
+  </si>
+  <si>
+    <t>8 runs for 5%. New normalisation meathod. Ideal (coherent, noiseless) Interferogram peaks are now set to 1.</t>
+  </si>
+  <si>
+    <t>15 runs for 5%</t>
+  </si>
+  <si>
+    <t>324 runs for 5%</t>
+  </si>
+  <si>
+    <t>501 runs for 5%</t>
+  </si>
+  <si>
+    <t>218 runs for 5%</t>
   </si>
 </sst>
 </file>
@@ -178,6 +196,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -482,25 +504,25 @@
   <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,7 +533,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -534,7 +556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -557,7 +579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -580,7 +602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -603,7 +625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -626,7 +648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -649,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -672,7 +694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
@@ -686,7 +708,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -712,16 +734,16 @@
         <v>15</v>
       </c>
       <c r="J12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K12" t="s">
         <v>16</v>
       </c>
       <c r="L12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>18</v>
       </c>
@@ -752,8 +774,11 @@
       <c r="K13">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>19</v>
       </c>
@@ -784,10 +809,13 @@
       <c r="K14">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>400</v>
@@ -817,12 +845,12 @@
         <v>20</v>
       </c>
       <c r="L15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>400</v>
@@ -851,10 +879,13 @@
       <c r="K16">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17">
         <v>400</v>
@@ -883,10 +914,13 @@
       <c r="K17">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18">
         <v>400</v>
@@ -915,10 +949,13 @@
       <c r="K18">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19">
         <v>400</v>
@@ -947,10 +984,13 @@
       <c r="K19">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20">
         <v>400</v>
@@ -979,10 +1019,13 @@
       <c r="K20">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21">
         <v>400</v>
@@ -1010,6 +1053,9 @@
       </c>
       <c r="K21">
         <v>20</v>
+      </c>
+      <c r="L21" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2D interferograms with convolution
</commit_message>
<xml_diff>
--- a/compressed_sensing/data/metadata.xlsx
+++ b/compressed_sensing/data/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/compressed_sensing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE315AF7-4761-4CDA-9D2C-372E6DDCACC3}"/>
+  <xr:revisionPtr revIDLastSave="228" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09759980-1814-4379-9D76-1CCBAE127108}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -114,9 +114,6 @@
     <t>1dmockanderrors9.csv</t>
   </si>
   <si>
-    <t>484 runs for 5%</t>
-  </si>
-  <si>
     <t>27 runs for 5%</t>
   </si>
   <si>
@@ -126,13 +123,13 @@
     <t>15 runs for 5%</t>
   </si>
   <si>
-    <t>324 runs for 5%</t>
-  </si>
-  <si>
     <t>501 runs for 5%</t>
   </si>
   <si>
-    <t>218 runs for 5%</t>
+    <t>1dmockanderrors10.csv</t>
+  </si>
+  <si>
+    <t>errorVSsamples done</t>
   </si>
 </sst>
 </file>
@@ -219,8 +216,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B0422EBC-0E69-4D8E-B10C-AB12EDC2789D}" name="Table4" displayName="Table4" ref="B12:L21" totalsRowShown="0">
-  <autoFilter ref="B12:L21" xr:uid="{B0422EBC-0E69-4D8E-B10C-AB12EDC2789D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B0422EBC-0E69-4D8E-B10C-AB12EDC2789D}" name="Table4" displayName="Table4" ref="B12:L22" totalsRowShown="0">
+  <autoFilter ref="B12:L22" xr:uid="{B0422EBC-0E69-4D8E-B10C-AB12EDC2789D}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{77F589C9-5F6B-46DA-9EEE-F5DBA498B0C1}" name="name"/>
     <tableColumn id="2" xr3:uid="{E2EBA6EE-B0E4-4DBE-AC80-C9B804CE497A}" name="array length (pixels)"/>
@@ -501,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L21"/>
+  <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +772,7 @@
         <v>20</v>
       </c>
       <c r="L13" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
@@ -810,7 +807,7 @@
         <v>20</v>
       </c>
       <c r="L14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -845,7 +842,7 @@
         <v>20</v>
       </c>
       <c r="L15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -880,7 +877,7 @@
         <v>20</v>
       </c>
       <c r="L16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
@@ -915,7 +912,7 @@
         <v>20</v>
       </c>
       <c r="L17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
@@ -950,7 +947,7 @@
         <v>20</v>
       </c>
       <c r="L18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
@@ -1020,7 +1017,7 @@
         <v>20</v>
       </c>
       <c r="L20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
@@ -1055,6 +1052,41 @@
         <v>20</v>
       </c>
       <c r="L21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22">
+        <v>400</v>
+      </c>
+      <c r="D22">
+        <v>50</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>0.3</v>
+      </c>
+      <c r="G22">
+        <v>60</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>20</v>
+      </c>
+      <c r="K22">
+        <v>20</v>
+      </c>
+      <c r="L22" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated 2D CS (v26)
</commit_message>
<xml_diff>
--- a/compressed_sensing/data/metadata.xlsx
+++ b/compressed_sensing/data/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/compressed_sensing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="228" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09759980-1814-4379-9D76-1CCBAE127108}"/>
+  <xr:revisionPtr revIDLastSave="254" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{134AC2DD-A862-405B-A29C-55678E6D1181}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -130,6 +130,21 @@
   </si>
   <si>
     <t>errorVSsamples done</t>
+  </si>
+  <si>
+    <t>2dmock.fits</t>
+  </si>
+  <si>
+    <t>vibration noise (mm)</t>
+  </si>
+  <si>
+    <t>read noise (% of peak)</t>
+  </si>
+  <si>
+    <t>2dmock1.fits</t>
+  </si>
+  <si>
+    <t>array height (pixels)</t>
   </si>
 </sst>
 </file>
@@ -230,6 +245,26 @@
     <tableColumn id="9" xr3:uid="{B4A3E234-74BF-4867-B948-7F0DE5726339}" name="read noise (% of coherant peak)"/>
     <tableColumn id="10" xr3:uid="{77B3527C-BD8A-4C2C-8196-7B026BA790D4}" name="averages"/>
     <tableColumn id="11" xr3:uid="{0756F483-F570-44BA-B1CF-32B491B94B5C}" name="Comments"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92CD28AF-F362-4617-ADAF-D33AF22B272F}" name="Table42" displayName="Table42" ref="B25:L27" totalsRowShown="0">
+  <autoFilter ref="B25:L27" xr:uid="{92CD28AF-F362-4617-ADAF-D33AF22B272F}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{6719D870-4E46-4962-A0E1-7C36966E4B06}" name="name"/>
+    <tableColumn id="2" xr3:uid="{4CF95376-0E4E-4CCD-8C41-9A67C4E9D0D7}" name="array length (pixels)"/>
+    <tableColumn id="11" xr3:uid="{4C9671E0-5374-404F-BBB4-B5AF4E08A121}" name="array height (pixels)"/>
+    <tableColumn id="3" xr3:uid="{1BBA310D-B794-467B-837D-096951889A16}" name="pixel pitch (um)"/>
+    <tableColumn id="4" xr3:uid="{24975619-0D77-4896-AB1C-9AA24BCD7BEB}" name="central frequency (THz)"/>
+    <tableColumn id="5" xr3:uid="{EEF530BC-5EB2-4BDD-8D71-77ADB6857F2F}" name="FWHM (THz)"/>
+    <tableColumn id="6" xr3:uid="{7D217B4F-808A-4344-BDD1-83D644E264D0}" name="theta (arcminutes)"/>
+    <tableColumn id="7" xr3:uid="{3D390970-BC28-40CF-85CB-FB4F4CEE69A2}" name="vibration noise (mm)"/>
+    <tableColumn id="8" xr3:uid="{5B764E25-5419-4784-AA71-F0975A966B32}" name="read noise (% of peak)"/>
+    <tableColumn id="9" xr3:uid="{01B81092-7B9A-4D17-AB21-F7E85B834DF3}" name="averages"/>
+    <tableColumn id="10" xr3:uid="{EF588157-60F7-4488-85F6-C66C07AFD41A}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -498,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L22"/>
+  <dimension ref="B1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,15 +1125,98 @@
         <v>34</v>
       </c>
     </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" t="s">
+        <v>36</v>
+      </c>
+      <c r="J25" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26">
+        <v>200</v>
+      </c>
+      <c r="D26">
+        <v>150</v>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26">
+        <v>30</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>10</v>
+      </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B24:K24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>